<commit_message>
Adding general information of the used environmental impact models, adding Readme.md and cosmetic code changes.
</commit_message>
<xml_diff>
--- a/data/conventional_power_10.xlsx
+++ b/data/conventional_power_10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\PycharmProjects\pythonProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481D5D0C-3889-4840-B7A1-A6281D2751C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8D7D3C-CA8D-45FF-89CF-D579B54521E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alpha" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="v" sheetId="8" r:id="rId8"/>
     <sheet name="w" sheetId="9" r:id="rId9"/>
     <sheet name="valid_ranges" sheetId="10" r:id="rId10"/>
+    <sheet name="general_info" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="136">
   <si>
     <r>
       <t>β</t>
@@ -2431,13 +2432,73 @@
       </rPr>
       <t/>
     </r>
+  </si>
+  <si>
+    <t>Model source:</t>
+  </si>
+  <si>
+    <t>Paulillo et al. (2022)</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.cesys.2022.100086</t>
+  </si>
+  <si>
+    <t>Equations 1-8 for model definition</t>
+  </si>
+  <si>
+    <t>Note that in equation 4, SR_p*beta_3,k+W_d*beta_4,k needs to be replaced by  W_d*beta_3,k+SR_p*beta_4,k; personal communication A. Paulillo, 2024-09-12</t>
+  </si>
+  <si>
+    <t>Coefficients from supplementary information</t>
+  </si>
+  <si>
+    <t>Paulillo et al. (2021)</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.cesys.2021.100054</t>
+  </si>
+  <si>
+    <t>Table 1 for valid ranges of parameters</t>
+  </si>
+  <si>
+    <t>Parameters:</t>
+  </si>
+  <si>
+    <t>Name for Code</t>
+  </si>
+  <si>
+    <t>Long Name (for error messages)</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>kgCO2/kWh</t>
+  </si>
+  <si>
+    <t>kgCH4/kWh</t>
+  </si>
+  <si>
+    <t>MW/well</t>
+  </si>
+  <si>
+    <t>m/well</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2495,6 +2556,31 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2513,10 +2599,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2539,8 +2626,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3402,7 +3493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567DC862-C7F7-48DA-99EF-AFC3F80D5034}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
@@ -3714,6 +3805,262 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF48D7B-F644-4C3F-AF0D-A39EC610B416}">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="6"/>
+      <c r="D25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{3066B7B0-44EE-45A6-83A0-53EFCE3693EB}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{D064709A-6F56-41E3-8770-CCB632741B73}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>